<commit_message>
updated the code to handle the wait
</commit_message>
<xml_diff>
--- a/Parallel_Test/Executor.xlsx
+++ b/Parallel_Test/Executor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NIMIT/eclipse-workspace/Parallel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NIMIT/git/Parallel_Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,7 +638,7 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -658,7 +658,7 @@
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -698,7 +698,7 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated changes for v2
</commit_message>
<xml_diff>
--- a/Parallel_Test/Executor.xlsx
+++ b/Parallel_Test/Executor.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>S.No</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>TC_05</t>
-  </si>
-  <si>
-    <t>TD3</t>
   </si>
   <si>
     <t>TC_06</t>
@@ -533,12 +530,13 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -569,7 +567,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -578,7 +576,7 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -598,7 +596,7 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -609,16 +607,16 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -629,16 +627,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -652,13 +650,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -666,19 +664,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -686,19 +684,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -706,7 +704,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -718,7 +716,7 @@
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting changes to avoid the thread overwrite for test data values
</commit_message>
<xml_diff>
--- a/Parallel_Test/Executor.xlsx
+++ b/Parallel_Test/Executor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NIMIT/git/Parallel_Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7D7A9DE8-AEED-5D42-AB5E-5F83751E2F45}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7DDC9B09-2B27-E24B-8AB5-BB7502F884DE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -546,7 +546,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,7 +723,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
@@ -732,7 +732,7 @@
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>